<commit_message>
Added comment to the documentation
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="141">
   <si>
     <t>Блок</t>
   </si>
@@ -126,9 +126,6 @@
     <t>ТС-37. Сброс заявки, находящаяся в статусе "В работе" , в которой "Автор" и "Исполнитель" заявки совпадают, во вкладке "Заявки" мобильного приложения "Мобильный хоспис"(Негативный)</t>
   </si>
   <si>
-    <t>ТС-38. Исполнения заявки, находящаяся в статусе "В работе", в которой "Автоор" и "Исполнитель" заявки совпадают, во вкладке "Заявки" мобильного приложения "Мобильный хоспис"(Позитивный</t>
-  </si>
-  <si>
     <t>ТС-39. Исполнения заявки, находящаяся в статусе "В работе", в которой "Автоор" и "Исполнитель" заявки совпадают, во вкладке "Заявки" мобильного приложения "Мобильный хоспис" (Негативный)</t>
   </si>
   <si>
@@ -387,50 +384,68 @@
     <t>Пройден</t>
   </si>
   <si>
+    <t>Высокий</t>
+  </si>
+  <si>
+    <t>ТС-13. Переход во вкладку "Все Заявки" через главное меню мобильного приложения "Мобильный хоспис"(Позитивный)</t>
+  </si>
+  <si>
+    <t>ТС-12. Переход во вкладку "Все Новости" через главное меню мобильного приложения "Мобильный хоспис"(Позитивный)</t>
+  </si>
+  <si>
+    <t>ТС-11. Поле "Пароль" состоит из букв разного регистра, при авторизации, в мобильном приложении "Мобильный хоспис"(Негативный)</t>
+  </si>
+  <si>
+    <t>ТС-10. Поле "Пароль" состоит из одного символа, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
+  </si>
+  <si>
+    <t>ТС-9. Поле "Пароль" состоит из спецсимволов, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
+  </si>
+  <si>
+    <t>ТС-8. Поле "Пароль" заполнено данными незарегистрированного пользователя, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
+  </si>
+  <si>
+    <t>ТС-7. Поле "Пароль" пустое, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
+  </si>
+  <si>
+    <t>ТС-6. Поле "Логин" состоит из букв разного регистра, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
+  </si>
+  <si>
+    <t>ТС-5. Поле "Логин" состоит из одного символа, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
+  </si>
+  <si>
+    <t>ТС-4. Поле "Логин" состоит из спецсимволов, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
+  </si>
+  <si>
+    <t>ТС-3. Поле "Логин" заполнено данными незарегистрированного пользователя, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
+  </si>
+  <si>
+    <t>ТС-2. Поле "Логин" пустое, при авторизации в мобильном приложении "Мобильный хоспис" (Негативный)</t>
+  </si>
+  <si>
+    <t>ТС-1. Авторизация в мобильном приложении "Мобильный хоспис" (Позитивный)</t>
+  </si>
+  <si>
     <t>Не пройден
-(найден дефект)</t>
-  </si>
-  <si>
-    <t>Высокий</t>
-  </si>
-  <si>
-    <t>ТС-13. Переход во вкладку "Все Заявки" через главное меню мобильного приложения "Мобильный хоспис"(Позитивный)</t>
-  </si>
-  <si>
-    <t>ТС-12. Переход во вкладку "Все Новости" через главное меню мобильного приложения "Мобильный хоспис"(Позитивный)</t>
-  </si>
-  <si>
-    <t>ТС-11. Поле "Пароль" состоит из букв разного регистра, при авторизации, в мобильном приложении "Мобильный хоспис"(Негативный)</t>
-  </si>
-  <si>
-    <t>ТС-10. Поле "Пароль" состоит из одного символа, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
-  </si>
-  <si>
-    <t>ТС-9. Поле "Пароль" состоит из спецсимволов, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
-  </si>
-  <si>
-    <t>ТС-8. Поле "Пароль" заполнено данными незарегистрированного пользователя, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
-  </si>
-  <si>
-    <t>ТС-7. Поле "Пароль" пустое, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
-  </si>
-  <si>
-    <t>ТС-6. Поле "Логин" состоит из букв разного регистра, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
-  </si>
-  <si>
-    <t>ТС-5. Поле "Логин" состоит из одного символа, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
-  </si>
-  <si>
-    <t>ТС-4. Поле "Логин" состоит из спецсимволов, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
-  </si>
-  <si>
-    <t>ТС-3. Поле "Логин" заполнено данными незарегистрированного пользователя, при авторизации в мобильном приложении "Мобильный хоспис"(Негативный)</t>
-  </si>
-  <si>
-    <t>ТС-2. Поле "Логин" пустое, при авторизации в мобильном приложении "Мобильный хоспис" (Негативный)</t>
-  </si>
-  <si>
-    <t>ТС-1. Авторизация в мобильном приложении "Мобильный хоспис" (Позитивный)</t>
+(найден дефект:  "Условия политики конфиденциальности не отображаются на экране")</t>
+  </si>
+  <si>
+    <t>Не пройден
+(найден дефект: "Пользовательское соглашение не отображается на экране")</t>
+  </si>
+  <si>
+    <t>Будет автоматизирован</t>
+  </si>
+  <si>
+    <t>Не будет автоматизирован
+Причина: "Элемент не кликабелен"</t>
+  </si>
+  <si>
+    <t>ТС-38. Исполнения заявки, находящаяся в статусе "В работе", в которой "Автор" и "Исполнитель" заявки совпадают, во вкладке "Заявки" мобильного приложения "Мобильный хоспис"(Позитивный</t>
+  </si>
+  <si>
+    <t>Будет автоматизирован.
+Найден дефект</t>
   </si>
 </sst>
 </file>
@@ -488,7 +503,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -762,56 +777,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -849,16 +819,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -868,6 +829,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -904,30 +889,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1212,15 +1173,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="C71" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="15" customWidth="1"/>
     <col min="4" max="4" width="41.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
@@ -1251,1233 +1212,1383 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="14"/>
-    </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="34"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="17" t="s">
+      <c r="E13" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C14" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="17" t="s">
+      <c r="D14" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="29" t="s">
+      <c r="C15" s="14" t="s">
         <v>63</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>64</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G15" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="17" t="s">
-        <v>65</v>
+      <c r="A16" s="26"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G16" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="17" t="s">
-        <v>66</v>
+      <c r="A17" s="26"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G17" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="17" t="s">
-        <v>67</v>
+      <c r="A18" s="26"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G18" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="23" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="28" t="s">
         <v>68</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>67</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G19" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G20" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G21" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G22" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G23" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
       <c r="D24" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G24" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
       <c r="D25" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G25" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
       <c r="D26" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G26" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G27" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
       <c r="D28" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G28" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
       <c r="D29" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G29" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="21"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="24"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G30" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="21"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="17" t="s">
-        <v>70</v>
+      <c r="A31" s="26"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G31" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="17" t="s">
-        <v>71</v>
+      <c r="A32" s="26"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="14" t="s">
+        <v>70</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G32" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="21"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="17" t="s">
-        <v>72</v>
+      <c r="A33" s="26"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="14" t="s">
+        <v>71</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G33" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="23" t="s">
-        <v>73</v>
+      <c r="A34" s="26"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="28" t="s">
+        <v>72</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G34" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
       <c r="D35" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G35" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="21"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="24"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="29"/>
       <c r="D36" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G36" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="23" t="s">
-        <v>74</v>
+      <c r="A37" s="26"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="28" t="s">
+        <v>73</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G37" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="21"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="24"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="29"/>
       <c r="D38" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G38" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="23" t="s">
-        <v>75</v>
+      <c r="A39" s="26"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="28" t="s">
+        <v>74</v>
       </c>
       <c r="D39" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="27"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G39" s="14"/>
-    </row>
-    <row r="40" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="22"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="6" t="s">
+      <c r="E40" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="B41" s="23" t="s">
+      <c r="E41" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="32"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="32"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="32"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="32"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="32"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="32"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="32"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="32"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="32"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="32"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="32"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="32"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="32"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="32"/>
+      <c r="B55" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G41" s="14"/>
-    </row>
-    <row r="42" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="27"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G42" s="14"/>
-    </row>
-    <row r="43" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="27"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G43" s="14"/>
-    </row>
-    <row r="44" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="27"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G44" s="14"/>
-    </row>
-    <row r="45" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="27"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G45" s="14"/>
-    </row>
-    <row r="46" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="27"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G46" s="14"/>
-    </row>
-    <row r="47" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="27"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G47" s="14"/>
-    </row>
-    <row r="48" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="27"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G48" s="14"/>
-    </row>
-    <row r="49" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="27"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G49" s="14"/>
-    </row>
-    <row r="50" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="27"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G50" s="14"/>
-    </row>
-    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="27"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G51" s="14"/>
-    </row>
-    <row r="52" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="27"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G52" s="14"/>
-    </row>
-    <row r="53" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A53" s="27"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G53" s="14"/>
-    </row>
-    <row r="54" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="27"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="6" t="s">
+      <c r="D55" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E54" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G54" s="14"/>
-    </row>
-    <row r="55" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="27"/>
-      <c r="B55" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="C55" s="17" t="s">
+      <c r="E55" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="32"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D56" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E55" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G55" s="14"/>
-    </row>
-    <row r="56" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="27"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="17" t="s">
+      <c r="E56" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="32"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E56" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G56" s="14"/>
-    </row>
-    <row r="57" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="27"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="17" t="s">
+      <c r="E57" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="32"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D58" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E57" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G57" s="14"/>
-    </row>
-    <row r="58" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="27"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="17" t="s">
+      <c r="E58" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="32"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D59" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E58" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G58" s="14"/>
-    </row>
-    <row r="59" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="27"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="17" t="s">
+      <c r="E59" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="32"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D60" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E59" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G59" s="14"/>
-    </row>
-    <row r="60" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="27"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="17" t="s">
+      <c r="E60" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="32"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D61" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E60" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G60" s="14"/>
-    </row>
-    <row r="61" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="27"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="17" t="s">
+      <c r="E61" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="32"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D62" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D61" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G61" s="14"/>
-    </row>
-    <row r="62" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A62" s="27"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="D62" s="6" t="s">
+      <c r="E62" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A63" s="32"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E62" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G62" s="14"/>
-    </row>
-    <row r="63" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A63" s="27"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="6" t="s">
+      <c r="E63" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A64" s="32"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E63" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G63" s="14"/>
-    </row>
-    <row r="64" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A64" s="27"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="6" t="s">
+      <c r="E64" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="32"/>
+      <c r="B65" s="30"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E64" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G64" s="14"/>
-    </row>
-    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A65" s="27"/>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="6" t="s">
+      <c r="E65" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A66" s="32"/>
+      <c r="B66" s="30"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E65" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G65" s="14"/>
-    </row>
-    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="27"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="6" t="s">
+      <c r="E66" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A67" s="32"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E66" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G66" s="14"/>
-    </row>
-    <row r="67" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A67" s="27"/>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="6" t="s">
+      <c r="E67" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A68" s="32"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E67" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G67" s="14"/>
-    </row>
-    <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A68" s="27"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="6" t="s">
+      <c r="E68" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A69" s="32"/>
+      <c r="B69" s="30"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E68" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G68" s="14"/>
-    </row>
-    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A69" s="27"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="6" t="s">
+      <c r="E69" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" s="32"/>
+      <c r="B70" s="30"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E69" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G69" s="14"/>
-    </row>
-    <row r="70" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A70" s="27"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="6" t="s">
+      <c r="E70" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A71" s="32"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E70" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G70" s="14"/>
-    </row>
-    <row r="71" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A71" s="27"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="6" t="s">
+      <c r="E71" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A72" s="32"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E71" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G71" s="14"/>
-    </row>
-    <row r="72" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A72" s="27"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="6" t="s">
+      <c r="E72" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="33"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E72" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G72" s="14"/>
-    </row>
-    <row r="73" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="28"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="24"/>
-      <c r="D73" s="6" t="s">
+      <c r="E73" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D74" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E73" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G73" s="14"/>
-    </row>
-    <row r="74" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="D74" s="15" t="s">
+      <c r="E74" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B75" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="C75" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D75" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E74" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G74" s="14"/>
-    </row>
-    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A75" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B75" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="C75" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="D75" s="6" t="s">
+      <c r="E75" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="27"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E75" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G75" s="14"/>
-    </row>
-    <row r="76" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="22"/>
-      <c r="B76" s="24"/>
-      <c r="C76" s="24"/>
-      <c r="D76" s="9" t="s">
-        <v>111</v>
-      </c>
       <c r="E76" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G76" s="16"/>
+        <v>136</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
@@ -5658,11 +5769,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A40"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="C53:C54"/>
@@ -5679,6 +5785,11 @@
     <mergeCell ref="C34:C36"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="C39:C40"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added changes cases and check
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="138">
   <si>
     <t>Блок</t>
   </si>
@@ -434,18 +434,7 @@
 (найден дефект: "Пользовательское соглашение не отображается на экране")</t>
   </si>
   <si>
-    <t>Будет автоматизирован</t>
-  </si>
-  <si>
-    <t>Не будет автоматизирован
-Причина: "Элемент не кликабелен"</t>
-  </si>
-  <si>
     <t>ТС-38. Исполнения заявки, находящаяся в статусе "В работе", в которой "Автор" и "Исполнитель" заявки совпадают, во вкладке "Заявки" мобильного приложения "Мобильный хоспис"(Позитивный</t>
-  </si>
-  <si>
-    <t>Будет автоматизирован.
-Найден дефект</t>
   </si>
 </sst>
 </file>
@@ -831,30 +820,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -889,6 +854,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1173,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C71" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,13 +1201,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="32" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="11" t="s">
@@ -1230,14 +1219,12 @@
       <c r="F2" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="6" t="s">
         <v>133</v>
       </c>
@@ -1247,14 +1234,12 @@
       <c r="F3" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="6" t="s">
         <v>132</v>
       </c>
@@ -1264,14 +1249,12 @@
       <c r="F4" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="6" t="s">
         <v>131</v>
       </c>
@@ -1281,14 +1264,12 @@
       <c r="F5" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="6" t="s">
         <v>130</v>
       </c>
@@ -1298,14 +1279,12 @@
       <c r="F6" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="23"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="6" t="s">
         <v>129</v>
       </c>
@@ -1315,14 +1294,12 @@
       <c r="F7" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="20" t="s">
+      <c r="A8" s="30"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="32" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -1334,14 +1311,12 @@
       <c r="F8" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
       <c r="D9" s="6" t="s">
         <v>127</v>
       </c>
@@ -1351,14 +1326,12 @@
       <c r="F9" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="6" t="s">
         <v>126</v>
       </c>
@@ -1368,14 +1341,12 @@
       <c r="F10" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="6" t="s">
         <v>125</v>
       </c>
@@ -1385,14 +1356,12 @@
       <c r="F11" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="6" t="s">
         <v>124</v>
       </c>
@@ -1402,12 +1371,10 @@
       <c r="F12" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="29" t="s">
         <v>57</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -1425,12 +1392,10 @@
       <c r="F13" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="14" t="s">
         <v>59</v>
       </c>
@@ -1446,15 +1411,13 @@
       <c r="F14" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="26" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -1469,13 +1432,11 @@
       <c r="F15" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="14" t="s">
         <v>64</v>
       </c>
@@ -1488,13 +1449,11 @@
       <c r="F16" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="14" t="s">
         <v>65</v>
       </c>
@@ -1507,13 +1466,11 @@
       <c r="F17" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
-      <c r="B18" s="36"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="14" t="s">
         <v>66</v>
       </c>
@@ -1526,16 +1483,14 @@
       <c r="F18" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="28" t="s">
+      <c r="A19" s="18"/>
+      <c r="B19" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="20" t="s">
         <v>67</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -1547,14 +1502,12 @@
       <c r="F19" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="6" t="s">
         <v>16</v>
       </c>
@@ -1564,14 +1517,12 @@
       <c r="F20" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="6" t="s">
         <v>17</v>
       </c>
@@ -1581,14 +1532,12 @@
       <c r="F21" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
       <c r="D22" s="6" t="s">
         <v>18</v>
       </c>
@@ -1598,14 +1547,12 @@
       <c r="F22" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="6" t="s">
         <v>19</v>
       </c>
@@ -1615,14 +1562,12 @@
       <c r="F23" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="6" t="s">
         <v>20</v>
       </c>
@@ -1632,14 +1577,12 @@
       <c r="F24" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="6" t="s">
         <v>21</v>
       </c>
@@ -1649,14 +1592,12 @@
       <c r="F25" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G25" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="6" t="s">
         <v>22</v>
       </c>
@@ -1666,14 +1607,12 @@
       <c r="F26" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="6" t="s">
         <v>23</v>
       </c>
@@ -1683,14 +1622,12 @@
       <c r="F27" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G27" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="6" t="s">
         <v>24</v>
       </c>
@@ -1700,14 +1637,12 @@
       <c r="F28" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G28" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="6" t="s">
         <v>25</v>
       </c>
@@ -1717,14 +1652,12 @@
       <c r="F29" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G29" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="29"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="21"/>
       <c r="D30" s="6" t="s">
         <v>26</v>
       </c>
@@ -1734,13 +1667,11 @@
       <c r="F30" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G30" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
-      <c r="B31" s="30"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="14" t="s">
         <v>69</v>
       </c>
@@ -1753,13 +1684,11 @@
       <c r="F31" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="26"/>
-      <c r="B32" s="30"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="14" t="s">
         <v>70</v>
       </c>
@@ -1772,13 +1701,11 @@
       <c r="F32" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G32" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
-      <c r="B33" s="30"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="14" t="s">
         <v>71</v>
       </c>
@@ -1791,14 +1718,12 @@
       <c r="F33" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G33" s="7"/>
     </row>
     <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="28" t="s">
+      <c r="A34" s="18"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="20" t="s">
         <v>72</v>
       </c>
       <c r="D34" s="6" t="s">
@@ -1810,14 +1735,12 @@
       <c r="F34" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G34" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
+      <c r="A35" s="18"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="6" t="s">
         <v>31</v>
       </c>
@@ -1827,14 +1750,12 @@
       <c r="F35" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G35" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="26"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="29"/>
+      <c r="A36" s="18"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="6" t="s">
         <v>32</v>
       </c>
@@ -1844,14 +1765,12 @@
       <c r="F36" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G36" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="28" t="s">
+      <c r="A37" s="18"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="20" t="s">
         <v>73</v>
       </c>
       <c r="D37" s="6" t="s">
@@ -1863,14 +1782,12 @@
       <c r="F37" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G37" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="29"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="21"/>
       <c r="D38" s="6" t="s">
         <v>34</v>
       </c>
@@ -1880,18 +1797,16 @@
       <c r="F38" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G38" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="28" t="s">
+      <c r="A39" s="18"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="20" t="s">
         <v>74</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>121</v>
@@ -1899,14 +1814,12 @@
       <c r="F39" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G39" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="27"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
       <c r="D40" s="6" t="s">
         <v>35</v>
       </c>
@@ -1916,15 +1829,13 @@
       <c r="F40" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G40" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G40" s="7"/>
     </row>
     <row r="41" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="20" t="s">
         <v>88</v>
       </c>
       <c r="C41" s="14" t="s">
@@ -1939,13 +1850,11 @@
       <c r="F41" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G41" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="32"/>
-      <c r="B42" s="30"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="22"/>
       <c r="C42" s="14" t="s">
         <v>77</v>
       </c>
@@ -1958,13 +1867,11 @@
       <c r="F42" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G42" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="32"/>
-      <c r="B43" s="30"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="14" t="s">
         <v>78</v>
       </c>
@@ -1977,13 +1884,11 @@
       <c r="F43" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G43" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="32"/>
-      <c r="B44" s="30"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="14" t="s">
         <v>79</v>
       </c>
@@ -1996,13 +1901,11 @@
       <c r="F44" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G44" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G44" s="7"/>
     </row>
     <row r="45" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="32"/>
-      <c r="B45" s="30"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="14" t="s">
         <v>80</v>
       </c>
@@ -2015,13 +1918,11 @@
       <c r="F45" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G45" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G45" s="7"/>
     </row>
     <row r="46" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="32"/>
-      <c r="B46" s="30"/>
+      <c r="A46" s="24"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="14" t="s">
         <v>81</v>
       </c>
@@ -2034,13 +1935,11 @@
       <c r="F46" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G46" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="32"/>
-      <c r="B47" s="30"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="22"/>
       <c r="C47" s="14" t="s">
         <v>82</v>
       </c>
@@ -2053,13 +1952,11 @@
       <c r="F47" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G47" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="32"/>
-      <c r="B48" s="30"/>
+      <c r="A48" s="24"/>
+      <c r="B48" s="22"/>
       <c r="C48" s="14" t="s">
         <v>83</v>
       </c>
@@ -2072,13 +1969,11 @@
       <c r="F48" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G48" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="32"/>
-      <c r="B49" s="30"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="22"/>
       <c r="C49" s="14" t="s">
         <v>84</v>
       </c>
@@ -2091,13 +1986,11 @@
       <c r="F49" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G49" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="32"/>
-      <c r="B50" s="30"/>
+      <c r="A50" s="24"/>
+      <c r="B50" s="22"/>
       <c r="C50" s="14" t="s">
         <v>85</v>
       </c>
@@ -2110,14 +2003,12 @@
       <c r="F50" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G50" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="28" t="s">
+      <c r="A51" s="24"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="20" t="s">
         <v>86</v>
       </c>
       <c r="D51" s="6" t="s">
@@ -2129,14 +2020,12 @@
       <c r="F51" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G51" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="32"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="29"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="21"/>
       <c r="D52" s="6" t="s">
         <v>47</v>
       </c>
@@ -2146,14 +2035,12 @@
       <c r="F52" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G52" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G52" s="7"/>
     </row>
     <row r="53" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="28" t="s">
+      <c r="A53" s="24"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="20" t="s">
         <v>87</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -2165,14 +2052,12 @@
       <c r="F53" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G53" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="32"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
       <c r="D54" s="6" t="s">
         <v>49</v>
       </c>
@@ -2182,13 +2067,11 @@
       <c r="F54" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G54" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G54" s="7"/>
     </row>
     <row r="55" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="32"/>
-      <c r="B55" s="28" t="s">
+      <c r="A55" s="24"/>
+      <c r="B55" s="20" t="s">
         <v>118</v>
       </c>
       <c r="C55" s="14" t="s">
@@ -2203,13 +2086,11 @@
       <c r="F55" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G55" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G55" s="7"/>
     </row>
     <row r="56" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="32"/>
-      <c r="B56" s="30"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="22"/>
       <c r="C56" s="14" t="s">
         <v>90</v>
       </c>
@@ -2222,13 +2103,11 @@
       <c r="F56" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G56" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G56" s="7"/>
     </row>
     <row r="57" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="32"/>
-      <c r="B57" s="30"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="22"/>
       <c r="C57" s="14" t="s">
         <v>91</v>
       </c>
@@ -2241,13 +2120,11 @@
       <c r="F57" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G57" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G57" s="7"/>
     </row>
     <row r="58" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="32"/>
-      <c r="B58" s="30"/>
+      <c r="A58" s="24"/>
+      <c r="B58" s="22"/>
       <c r="C58" s="14" t="s">
         <v>92</v>
       </c>
@@ -2260,13 +2137,11 @@
       <c r="F58" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G58" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G58" s="7"/>
     </row>
     <row r="59" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="32"/>
-      <c r="B59" s="30"/>
+      <c r="A59" s="24"/>
+      <c r="B59" s="22"/>
       <c r="C59" s="14" t="s">
         <v>93</v>
       </c>
@@ -2279,13 +2154,11 @@
       <c r="F59" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G59" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G59" s="7"/>
     </row>
     <row r="60" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="32"/>
-      <c r="B60" s="30"/>
+      <c r="A60" s="24"/>
+      <c r="B60" s="22"/>
       <c r="C60" s="14" t="s">
         <v>94</v>
       </c>
@@ -2298,13 +2171,11 @@
       <c r="F60" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G60" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G60" s="7"/>
     </row>
     <row r="61" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="32"/>
-      <c r="B61" s="30"/>
+      <c r="A61" s="24"/>
+      <c r="B61" s="22"/>
       <c r="C61" s="14" t="s">
         <v>95</v>
       </c>
@@ -2317,14 +2188,12 @@
       <c r="F61" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G61" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G61" s="7"/>
     </row>
     <row r="62" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A62" s="32"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="28" t="s">
+      <c r="A62" s="24"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="20" t="s">
         <v>117</v>
       </c>
       <c r="D62" s="6" t="s">
@@ -2336,14 +2205,12 @@
       <c r="F62" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G62" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G62" s="7"/>
     </row>
     <row r="63" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A63" s="32"/>
-      <c r="B63" s="30"/>
-      <c r="C63" s="30"/>
+      <c r="A63" s="24"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
       <c r="D63" s="6" t="s">
         <v>97</v>
       </c>
@@ -2353,14 +2220,12 @@
       <c r="F63" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G63" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G63" s="7"/>
     </row>
     <row r="64" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A64" s="32"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
+      <c r="A64" s="24"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
       <c r="D64" s="6" t="s">
         <v>98</v>
       </c>
@@ -2370,14 +2235,12 @@
       <c r="F64" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G64" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G64" s="7"/>
     </row>
     <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A65" s="32"/>
-      <c r="B65" s="30"/>
-      <c r="C65" s="30"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="22"/>
+      <c r="C65" s="22"/>
       <c r="D65" s="6" t="s">
         <v>99</v>
       </c>
@@ -2387,14 +2250,12 @@
       <c r="F65" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G65" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G65" s="7"/>
     </row>
     <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="32"/>
-      <c r="B66" s="30"/>
-      <c r="C66" s="30"/>
+      <c r="A66" s="24"/>
+      <c r="B66" s="22"/>
+      <c r="C66" s="22"/>
       <c r="D66" s="6" t="s">
         <v>100</v>
       </c>
@@ -2404,14 +2265,12 @@
       <c r="F66" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G66" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G66" s="7"/>
     </row>
     <row r="67" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A67" s="32"/>
-      <c r="B67" s="30"/>
-      <c r="C67" s="30"/>
+      <c r="A67" s="24"/>
+      <c r="B67" s="22"/>
+      <c r="C67" s="22"/>
       <c r="D67" s="6" t="s">
         <v>101</v>
       </c>
@@ -2421,14 +2280,12 @@
       <c r="F67" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G67" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G67" s="7"/>
     </row>
     <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A68" s="32"/>
-      <c r="B68" s="30"/>
-      <c r="C68" s="30"/>
+      <c r="A68" s="24"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
       <c r="D68" s="6" t="s">
         <v>102</v>
       </c>
@@ -2438,14 +2295,12 @@
       <c r="F68" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G68" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G68" s="7"/>
     </row>
     <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A69" s="32"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="30"/>
+      <c r="A69" s="24"/>
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
       <c r="D69" s="6" t="s">
         <v>103</v>
       </c>
@@ -2455,14 +2310,12 @@
       <c r="F69" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G69" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G69" s="7"/>
     </row>
     <row r="70" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A70" s="32"/>
-      <c r="B70" s="30"/>
-      <c r="C70" s="30"/>
+      <c r="A70" s="24"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
       <c r="D70" s="6" t="s">
         <v>104</v>
       </c>
@@ -2472,14 +2325,12 @@
       <c r="F70" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G70" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G70" s="7"/>
     </row>
     <row r="71" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A71" s="32"/>
-      <c r="B71" s="30"/>
-      <c r="C71" s="30"/>
+      <c r="A71" s="24"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
       <c r="D71" s="6" t="s">
         <v>105</v>
       </c>
@@ -2489,14 +2340,12 @@
       <c r="F71" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G71" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G71" s="7"/>
     </row>
     <row r="72" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A72" s="32"/>
-      <c r="B72" s="30"/>
-      <c r="C72" s="30"/>
+      <c r="A72" s="24"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
       <c r="D72" s="6" t="s">
         <v>106</v>
       </c>
@@ -2506,14 +2355,12 @@
       <c r="F72" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G72" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G72" s="7"/>
     </row>
     <row r="73" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="33"/>
-      <c r="B73" s="29"/>
-      <c r="C73" s="29"/>
+      <c r="A73" s="25"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="21"/>
       <c r="D73" s="6" t="s">
         <v>107</v>
       </c>
@@ -2523,9 +2370,7 @@
       <c r="F73" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G73" s="7" t="s">
-        <v>138</v>
-      </c>
+      <c r="G73" s="7"/>
     </row>
     <row r="74" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
@@ -2546,18 +2391,16 @@
       <c r="F74" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G74" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="G74" s="7"/>
     </row>
     <row r="75" spans="1:7" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="25" t="s">
+      <c r="A75" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B75" s="28" t="s">
+      <c r="B75" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C75" s="28" t="s">
+      <c r="C75" s="20" t="s">
         <v>113</v>
       </c>
       <c r="D75" s="6" t="s">
@@ -2569,14 +2412,12 @@
       <c r="F75" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="G75" s="7" t="s">
-        <v>140</v>
-      </c>
+      <c r="G75" s="7"/>
     </row>
     <row r="76" spans="1:7" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="27"/>
-      <c r="B76" s="29"/>
-      <c r="C76" s="29"/>
+      <c r="A76" s="19"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
       <c r="D76" s="9" t="s">
         <v>110</v>
       </c>
@@ -2586,9 +2427,7 @@
       <c r="F76" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="G76" s="7" t="s">
-        <v>140</v>
-      </c>
+      <c r="G76" s="7"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
@@ -5769,6 +5608,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A40"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="C53:C54"/>
@@ -5785,11 +5629,6 @@
     <mergeCell ref="C34:C36"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="C39:C40"/>
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>